<commit_message>
Multiple Tabs task in progress
</commit_message>
<xml_diff>
--- a/reschedule_sheet_small.xlsx
+++ b/reschedule_sheet_small.xlsx
@@ -479,10 +479,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C10"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="29.44" customWidth="1" style="3" min="1" max="1"/>
     <col width="23.61" customWidth="1" style="3" min="2" max="2"/>
@@ -543,11 +543,7 @@
           <t>Please dont call</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
+      <c r="C4" s="3" t="inlineStr"/>
     </row>
     <row r="5" ht="12.8" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr"/>
@@ -556,11 +552,7 @@
           <t>Next Week</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
+      <c r="C5" s="3" t="inlineStr"/>
     </row>
     <row r="6" ht="12.8" customHeight="1" s="4">
       <c r="A6" s="3" t="inlineStr"/>
@@ -593,7 +585,7 @@
       <c r="A9" s="3" t="inlineStr"/>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Day After tomorrow</t>
+          <t>2 Days After tomorrow</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr"/>

</xml_diff>

<commit_message>
made a bit fast
</commit_message>
<xml_diff>
--- a/reschedule_sheet_small.xlsx
+++ b/reschedule_sheet_small.xlsx
@@ -479,10 +479,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="29.44" customWidth="1" style="3" min="1" max="1"/>
     <col width="23.61" customWidth="1" style="3" min="2" max="2"/>
@@ -543,7 +543,11 @@
           <t>Please dont call</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr"/>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="12.8" customHeight="1" s="4">
       <c r="A5" s="3" t="inlineStr"/>

</xml_diff>